<commit_message>
Saved some open excel files
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/NSDIresults.xlsx
+++ b/distributed-tensorflow-simulator/NSDIresults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domenicbottini/PycharmProjects/networkml/distributed-tensorflow-simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDCD31C-2C27-694A-A9AD-8A292C17D9DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8539B24-649E-1E4F-AD44-4EC2A82074E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="4" xr2:uid="{92131C13-1580-C54C-971C-CEFD8DFC3C3E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{92131C13-1580-C54C-971C-CEFD8DFC3C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,50 @@
     <sheet name="Global Barrier" sheetId="7" r:id="rId9"/>
     <sheet name="Optimal Distr" sheetId="4" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Overall!$A$30:$A$35</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Overall!$B$29</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Overall!$C$29</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Overall!$C$30:$C$35</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Overall!$D$29</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Overall!$D$30:$D$35</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Overall!$A$30:$A$35</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Overall!$B$29</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Overall!$B$30:$B$35</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Overall!$C$29</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Overall!$C$30:$C$35</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Overall!$D$29</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Overall!$B$30:$B$35</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Overall!$D$30:$D$35</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Overall!$A$12:$A$17</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Overall!$B$11</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Overall!$B$12:$B$17</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Overall!$C$11</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Overall!$C$12:$C$17</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Overall!$D$11</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Overall!$D$12:$D$17</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Overall!$A$30:$A$35</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Overall!$B$29</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Overall!$C$29</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Overall!$B$30:$B$35</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Overall!$C$29</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Overall!$C$30:$C$35</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Overall!$D$29</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Overall!$D$30:$D$35</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Overall!$A$21:$A$26</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Overall!$B$20</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Overall!$B$21:$B$26</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Overall!$C$20</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Overall!$C$21:$C$26</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Overall!$C$30:$C$35</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Overall!$D$20</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Overall!$D$21:$D$26</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Overall!$D$29</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Overall!$D$30:$D$35</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Overall!$A$30:$A$35</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Overall!$B$29</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Overall!$B$30:$B$35</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="49">
   <si>
     <t>multiagg</t>
   </si>
@@ -178,12 +222,21 @@
   <si>
     <t>inception-v3 64</t>
   </si>
+  <si>
+    <t>32workers</t>
+  </si>
+  <si>
+    <t>multiagg no barier</t>
+  </si>
+  <si>
+    <t>ring-reduce</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1013,14 +1066,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110591626231223"/>
+          <c:x val="0.13617426536948526"/>
           <c:y val="4.3209406256650297E-2"/>
-          <c:w val="0.86579213760641505"/>
+          <c:w val="0.82232677344205563"/>
           <c:h val="0.67128197488827401"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1049,7 +1102,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$12:$A$17</c:f>
               <c:numCache>
@@ -1075,34 +1128,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$B$12:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.83758099702857103</c:v>
+                  <c:v>0.84399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83065642221714198</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81434819940571401</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82262642255238005</c:v>
+                  <c:v>0.82399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82062267113142795</c:v>
+                  <c:v>0.82199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81973470833371398</c:v>
+                  <c:v>0.82199999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1119,7 +1172,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>horovod</c:v>
+                  <c:v>ring-reduce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1137,7 +1190,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$12:$A$17</c:f>
               <c:numCache>
@@ -1163,34 +1216,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$C$12:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.03791462857141</c:v>
+                  <c:v>0.86899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82694563510855901</c:v>
+                  <c:v>0.82399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82447966500571002</c:v>
+                  <c:v>0.82599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82463125156570505</c:v>
+                  <c:v>0.82499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82441393444570898</c:v>
+                  <c:v>0.82699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82388994815999805</c:v>
+                  <c:v>0.82399999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1225,7 +1278,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$12:$A$17</c:f>
               <c:numCache>
@@ -1251,34 +1304,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$D$12:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4251641732571101</c:v>
+                  <c:v>1.4410000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.81783354514286299</c:v>
+                  <c:v>0.81899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81770324388571303</c:v>
+                  <c:v>0.82099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.811254563047618</c:v>
+                  <c:v>0.81799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81895876187428496</c:v>
+                  <c:v>0.81899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81895272144457099</c:v>
+                  <c:v>0.82099999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1294,14 +1347,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1778803632"/>
         <c:axId val="1778809664"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1778803632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="125"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1350,7 +1404,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.37140009047909045"/>
-              <c:y val="0.77910755258632725"/>
+              <c:y val="0.8048773724072642"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1397,8 +1451,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1415,7 +1469,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1432,12 +1486,9 @@
         </c:txPr>
         <c:crossAx val="1778809664"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="0"/>
-        <c:tickLblSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1778809664"/>
         <c:scaling>
@@ -1541,7 +1592,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1557,8 +1608,8 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1778803632"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1645,8 +1696,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.13433207119898541"/>
           <c:y val="0.87794349172265729"/>
-          <c:w val="0.8107418382510394"/>
-          <c:h val="8.0419450947010002E-2"/>
+          <c:w val="0.77524759453508452"/>
+          <c:h val="0.10022182787158199"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1736,14 +1787,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110591626231223"/>
+          <c:x val="0.12955941748494879"/>
           <c:y val="4.3209406256650297E-2"/>
-          <c:w val="0.86579213760641505"/>
+          <c:w val="0.82993648393874009"/>
           <c:h val="0.67128197488827401"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1772,7 +1823,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$21:$A$26</c:f>
               <c:numCache>
@@ -1798,34 +1849,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$B$21:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.66306217005714196</c:v>
+                  <c:v>0.66300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60076316543999997</c:v>
+                  <c:v>0.59799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57861586843428503</c:v>
+                  <c:v>0.57099999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54090009496380898</c:v>
+                  <c:v>0.55700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.561185077074285</c:v>
+                  <c:v>0.56200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53489891412114299</c:v>
+                  <c:v>0.55100000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1842,7 +1893,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>horovod</c:v>
+                  <c:v>ring-reduce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1860,7 +1911,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$21:$A$26</c:f>
               <c:numCache>
@@ -1886,34 +1937,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$C$21:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.82672751634284303</c:v>
+                  <c:v>0.64700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.56816687359998597</c:v>
+                  <c:v>0.55600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52665219803427898</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56459213769141803</c:v>
+                  <c:v>0.55200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56294679515427903</c:v>
+                  <c:v>0.55900000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56288154049828398</c:v>
+                  <c:v>0.55800000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1948,7 +1999,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$21:$A$26</c:f>
               <c:numCache>
@@ -1974,34 +2025,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$D$21:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.96845884297140405</c:v>
+                  <c:v>0.94699999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55807887652571397</c:v>
+                  <c:v>0.56399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55027469586285604</c:v>
+                  <c:v>0.55200000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55554025392761797</c:v>
+                  <c:v>0.55400000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55495877650285597</c:v>
+                  <c:v>0.55100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55609558092800004</c:v>
+                  <c:v>0.55300000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2017,14 +2068,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1778803632"/>
         <c:axId val="1778809664"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1778803632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="125"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2072,8 +2124,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.37653451607499711"/>
-              <c:y val="0.78197086589976472"/>
+              <c:x val="0.37816441278124369"/>
+              <c:y val="0.81060399903413916"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2120,8 +2172,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2138,7 +2190,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2155,12 +2207,9 @@
         </c:txPr>
         <c:crossAx val="1778809664"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="0"/>
-        <c:tickLblSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1778809664"/>
         <c:scaling>
@@ -2252,11 +2301,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2272,8 +2321,8 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1778803632"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2360,8 +2409,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.13090912080171427"/>
           <c:y val="0.87794349172265729"/>
-          <c:w val="0.8107418382510394"/>
-          <c:h val="8.0419450947010002E-2"/>
+          <c:w val="0.73831151746787937"/>
+          <c:h val="0.10022182787158199"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2451,14 +2500,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110591626231223"/>
+          <c:x val="0.15093648014776365"/>
           <c:y val="4.3209406256650297E-2"/>
-          <c:w val="0.86579213760641505"/>
+          <c:w val="0.81536888556955522"/>
           <c:h val="0.67128197488827401"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2487,7 +2536,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$30:$A$35</c:f>
               <c:numCache>
@@ -2513,34 +2562,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$B$30:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.60727629120000004</c:v>
+                  <c:v>0.60299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57530594505142796</c:v>
+                  <c:v>0.57299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56145868681142796</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55974769596952301</c:v>
+                  <c:v>0.55800000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56339220054857098</c:v>
+                  <c:v>0.55500000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56397890329599898</c:v>
+                  <c:v>0.55300000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2557,7 +2606,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>horovod</c:v>
+                  <c:v>ring-reduce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2575,7 +2624,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$30:$A$35</c:f>
               <c:numCache>
@@ -2601,34 +2650,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$C$30:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.69515517531427695</c:v>
+                  <c:v>0.56599999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57369752978285504</c:v>
+                  <c:v>0.55100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.560253569828561</c:v>
+                  <c:v>0.56100000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56605287558094597</c:v>
+                  <c:v>0.55600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.564735700479992</c:v>
+                  <c:v>0.56200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56647900101485105</c:v>
+                  <c:v>0.55800000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2663,7 +2712,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$30:$A$35</c:f>
               <c:numCache>
@@ -2689,34 +2738,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$D$30:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.57934792822856496</c:v>
+                  <c:v>0.56899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.560796773485714</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55521981531428499</c:v>
+                  <c:v>0.54700000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54578940068571302</c:v>
+                  <c:v>0.55400000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55564562194285605</c:v>
+                  <c:v>0.54800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56064506898285604</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2732,14 +2781,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1778803632"/>
         <c:axId val="1778809664"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1778803632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="125"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2787,8 +2837,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.410764010355186"/>
-              <c:y val="0.77910746967439903"/>
+              <c:x val="0.4107640200477084"/>
+              <c:y val="0.80774068572070168"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2835,8 +2885,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2853,7 +2903,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2870,17 +2920,15 @@
         </c:txPr>
         <c:crossAx val="1778809664"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="0"/>
-        <c:tickLblSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1778809664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.5"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.30000000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2971,7 +3019,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2987,8 +3035,8 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1778803632"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3075,8 +3123,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.13090912080171427"/>
           <c:y val="0.87794349172265729"/>
-          <c:w val="0.8107418382510394"/>
-          <c:h val="8.0419450947010002E-2"/>
+          <c:w val="0.77524759453508452"/>
+          <c:h val="0.10022182787158199"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -9847,7 +9895,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>horovod</c:v>
+                  <c:v>ring-reduce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19693,14 +19741,14 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.110591626231223"/>
+          <c:x val="0.13626374722239029"/>
           <c:y val="4.3209406256650297E-2"/>
-          <c:w val="0.86579213760641505"/>
+          <c:w val="0.84012005122566558"/>
           <c:h val="0.67128197488827401"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -19729,7 +19777,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$3:$A$8</c:f>
               <c:numCache>
@@ -19755,34 +19803,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9135307161600501</c:v>
+                  <c:v>1.9139999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76543523788801104</c:v>
+                  <c:v>0.76500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41805489280000901</c:v>
+                  <c:v>0.41799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.33511760008532598</c:v>
+                  <c:v>0.33500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.293647446400009</c:v>
+                  <c:v>0.29399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26942581447680702</c:v>
+                  <c:v>0.26900000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -19799,7 +19847,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>horovod</c:v>
+                  <c:v>ring-reduce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -19817,7 +19865,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$3:$A$8</c:f>
               <c:numCache>
@@ -19843,34 +19891,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>33.954211500809897</c:v>
+                  <c:v>1.4530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.688728600311901</c:v>
+                  <c:v>0.68300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9328343001559203</c:v>
+                  <c:v>0.42699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6814695334424297</c:v>
+                  <c:v>0.34300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5553871500779</c:v>
+                  <c:v>0.30099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.87965772006577</c:v>
+                  <c:v>0.27600000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -19905,7 +19953,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Overall!$A$3:$A$8</c:f>
               <c:numCache>
@@ -19931,34 +19979,34 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Overall!$D$3:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.4696218393598999</c:v>
+                  <c:v>3.47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4905966210560599</c:v>
+                  <c:v>1.4910000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83100617484804096</c:v>
+                  <c:v>0.83099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61138563754668596</c:v>
+                  <c:v>0.61099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50073379040002497</c:v>
+                  <c:v>0.501</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.43540864522237999</c:v>
+                  <c:v>0.435</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -19974,14 +20022,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="1778803632"/>
         <c:axId val="1778809664"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="1778803632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="125"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -20015,8 +20064,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.36626566488318374"/>
-              <c:y val="0.7848341792132022"/>
+              <c:x val="0.36626564318835481"/>
+              <c:y val="0.81060399903413916"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -20049,8 +20098,8 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -20067,7 +20116,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -20084,12 +20133,9 @@
         </c:txPr>
         <c:crossAx val="1778809664"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="0"/>
-        <c:tickLblSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="25"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="1778809664"/>
         <c:scaling>
@@ -20184,7 +20230,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -20200,8 +20246,8 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1778803632"/>
-        <c:crossesAt val="1"/>
-        <c:crossBetween val="between"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -20288,8 +20334,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.13090912080171427"/>
           <c:y val="0.87794349172265729"/>
-          <c:w val="0.8107418382510394"/>
-          <c:h val="8.0419450947010002E-2"/>
+          <c:w val="0.73831151746787937"/>
+          <c:h val="0.10022182787158199"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -37315,17 +37361,17 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView zoomScale="41" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -37339,7 +37385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>4</v>
       </c>
@@ -37356,7 +37402,7 @@
         <v>1.9029847929600501</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>8</v>
       </c>
@@ -37373,7 +37419,7 @@
         <v>1.8924493555200499</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>16</v>
       </c>
@@ -37390,7 +37436,7 @@
         <v>1.9029952787200499</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>32</v>
       </c>
@@ -37407,12 +37453,12 @@
         <v>1.9135307161600501</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -37426,7 +37472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
@@ -37443,7 +37489,7 @@
         <v>0.74885368243201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>8</v>
       </c>
@@ -37460,7 +37506,7 @@
         <v>0.75724269363201002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>16</v>
       </c>
@@ -37477,7 +37523,7 @@
         <v>0.75315061580801002</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>32</v>
       </c>
@@ -37494,12 +37540,12 @@
         <v>0.76543523788801104</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -37513,7 +37559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>4</v>
       </c>
@@ -37530,7 +37576,7 @@
         <v>0.84348572479999995</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>8</v>
       </c>
@@ -37547,7 +37593,7 @@
         <v>0.899146301714285</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>16</v>
       </c>
@@ -37564,7 +37610,7 @@
         <v>0.84700953919999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>32</v>
       </c>
@@ -37581,12 +37627,12 @@
         <v>0.83758099702857103</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>2</v>
       </c>
@@ -37600,7 +37646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>4</v>
       </c>
@@ -37617,7 +37663,7 @@
         <v>0.82541828991999899</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>8</v>
       </c>
@@ -37634,7 +37680,7 @@
         <v>0.88035885220571397</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>16</v>
       </c>
@@ -37651,7 +37697,7 @@
         <v>0.82808495853714204</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>32</v>
       </c>
@@ -37668,12 +37714,12 @@
         <v>0.83065642221714198</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>2</v>
       </c>
@@ -37687,7 +37733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>4</v>
       </c>
@@ -37704,7 +37750,7 @@
         <v>0.65891931291428496</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>8</v>
       </c>
@@ -37721,7 +37767,7 @@
         <v>0.53814719314285597</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>16</v>
       </c>
@@ -37738,7 +37784,7 @@
         <v>0.61479815771428503</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>32</v>
       </c>
@@ -37755,12 +37801,12 @@
         <v>0.66306217005714196</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="B42" t="s">
         <v>2</v>
       </c>
@@ -37774,7 +37820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4</v>
       </c>
@@ -37791,7 +37837,7 @@
         <v>0.59462029659428495</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>8</v>
       </c>
@@ -37808,7 +37854,7 @@
         <v>0.44390599917714202</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>16</v>
       </c>
@@ -37825,7 +37871,7 @@
         <v>0.56576315373714203</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>32</v>
       </c>
@@ -37842,12 +37888,12 @@
         <v>0.60076316543999997</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="B50" t="s">
         <v>2</v>
       </c>
@@ -37861,7 +37907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>4</v>
       </c>
@@ -37878,7 +37924,7 @@
         <v>0.54127629119999998</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>8</v>
       </c>
@@ -37895,7 +37941,7 @@
         <v>0.564847719771428</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>16</v>
       </c>
@@ -37912,7 +37958,7 @@
         <v>0.59184771977142803</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>32</v>
       </c>
@@ -37929,12 +37975,12 @@
         <v>0.60727629120000004</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="B58" t="s">
         <v>2</v>
       </c>
@@ -37948,7 +37994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>4</v>
       </c>
@@ -37965,7 +38011,7 @@
         <v>0.51173451648000001</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>8</v>
       </c>
@@ -37982,7 +38028,7 @@
         <v>0.53530594505142803</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>16</v>
       </c>
@@ -37999,7 +38045,7 @@
         <v>0.56444880219428495</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>32</v>
       </c>
@@ -38027,15 +38073,17 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>37</v>
       </c>
@@ -38049,7 +38097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -38066,7 +38114,7 @@
         <v>1.4905966210560599</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -38083,7 +38131,7 @@
         <v>1.7537265134080799</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -38100,7 +38148,7 @@
         <v>0.81783354514286299</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -38117,7 +38165,7 @@
         <v>0.875961843565775</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -38134,7 +38182,7 @@
         <v>0.55807887652571397</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -38151,7 +38199,7 @@
         <v>0.58144043958858005</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -38168,7 +38216,7 @@
         <v>0.560796773485714</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -38192,412 +38240,907 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1ABA06-43D5-D54D-8A82-C64B5A0E5D75}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
-        <v>1.9135307161600501</v>
+        <v>1.9139999999999999</v>
       </c>
       <c r="C3">
-        <v>33.954211500809897</v>
+        <v>1.4530000000000001</v>
       </c>
       <c r="D3">
-        <v>3.4696218393598999</v>
+        <v>3.47</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>25</v>
       </c>
       <c r="B4">
-        <v>0.76543523788801104</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="C4">
-        <v>13.688728600311901</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="D4">
-        <v>1.4905966210560599</v>
+        <v>1.4910000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>0.41805489280000901</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="C5">
-        <v>6.9328343001559203</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D5">
-        <v>0.83100617484804096</v>
+        <v>0.83099999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>75</v>
       </c>
       <c r="B6">
-        <v>0.33511760008532598</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="C6">
-        <v>4.6814695334424297</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="D6">
-        <v>0.61138563754668596</v>
+        <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>100</v>
       </c>
       <c r="B7">
-        <v>0.293647446400009</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="C7">
-        <v>3.5553871500779</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="D7">
-        <v>0.50073379040002497</v>
+        <v>0.501</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>125</v>
       </c>
       <c r="B8">
-        <v>0.26942581447680702</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="C8">
-        <v>2.87965772006577</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="D8">
-        <v>0.43540864522237999</v>
+        <v>0.435</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.83758099702857103</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="C12">
-        <v>1.03791462857141</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="D12">
-        <v>1.4251641732571101</v>
+        <v>1.4410000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13">
-        <v>0.83065642221714198</v>
+        <v>0.83</v>
       </c>
       <c r="C13">
-        <v>0.82694563510855901</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="D13">
-        <v>0.81783354514286299</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>50</v>
       </c>
       <c r="B14">
-        <v>0.81434819940571401</v>
+        <v>0.82</v>
       </c>
       <c r="C14">
-        <v>0.82447966500571002</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="D14">
-        <v>0.81770324388571303</v>
+        <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>75</v>
       </c>
       <c r="B15">
-        <v>0.82262642255238005</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="C15">
-        <v>0.82463125156570505</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="D15">
-        <v>0.811254563047618</v>
+        <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>100</v>
       </c>
       <c r="B16">
-        <v>0.82062267113142795</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="C16">
-        <v>0.82441393444570898</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="D16">
-        <v>0.81895876187428496</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>125</v>
       </c>
       <c r="B17">
-        <v>0.81973470833371398</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="C17">
-        <v>0.82388994815999805</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="D17">
-        <v>0.81895272144457099</v>
+        <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>10</v>
       </c>
       <c r="B21">
-        <v>0.66306217005714196</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="C21">
-        <v>0.82672751634284303</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="D21">
-        <v>0.96845884297140405</v>
+        <v>0.94699999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.60076316543999997</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="C22">
-        <v>0.56816687359998597</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="D22">
-        <v>0.55807887652571397</v>
+        <v>0.56399999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>50</v>
       </c>
       <c r="B23">
-        <v>0.57861586843428503</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="C23">
-        <v>0.52665219803427898</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D23">
-        <v>0.55027469586285604</v>
+        <v>0.55200000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>75</v>
       </c>
       <c r="B24">
-        <v>0.54090009496380898</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="C24">
-        <v>0.56459213769141803</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="D24">
-        <v>0.55554025392761797</v>
+        <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>100</v>
       </c>
       <c r="B25">
-        <v>0.561185077074285</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="C25">
-        <v>0.56294679515427903</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="D25">
-        <v>0.55495877650285597</v>
+        <v>0.55100000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>125</v>
       </c>
       <c r="B26">
-        <v>0.53489891412114299</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="C26">
-        <v>0.56288154049828398</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="D26">
-        <v>0.55609558092800004</v>
+        <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>10</v>
       </c>
       <c r="B30">
-        <v>0.60727629120000004</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="C30">
-        <v>0.69515517531427695</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="D30">
-        <v>0.57934792822856496</v>
+        <v>0.56899999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31">
-        <v>0.57530594505142796</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="C31">
-        <v>0.57369752978285504</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="D31">
-        <v>0.560796773485714</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>50</v>
       </c>
       <c r="B32">
-        <v>0.56145868681142796</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C32">
-        <v>0.560253569828561</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="D32">
-        <v>0.55521981531428499</v>
+        <v>0.54700000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>75</v>
       </c>
       <c r="B33">
-        <v>0.55974769596952301</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="C33">
-        <v>0.56605287558094597</v>
+        <v>0.55600000000000005</v>
       </c>
       <c r="D33">
-        <v>0.54578940068571302</v>
+        <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>100</v>
       </c>
       <c r="B34">
-        <v>0.56339220054857098</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C34">
-        <v>0.564735700479992</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="D34">
-        <v>0.55564562194285605</v>
+        <v>0.54800000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>125</v>
       </c>
       <c r="B35">
-        <v>0.56397890329599898</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="C35">
-        <v>0.56647900101485105</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="D35">
-        <v>0.56064506898285604</v>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>1.9135307161600501</v>
+      </c>
+      <c r="C43">
+        <v>1.4529618815999901</v>
+      </c>
+      <c r="D43">
+        <v>3.4696218393598999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>0.76543628646401096</v>
+      </c>
+      <c r="C44">
+        <v>0.683084752640014</v>
+      </c>
+      <c r="D44">
+        <v>1.4905819495680599</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>0.41805489280000901</v>
+      </c>
+      <c r="C45">
+        <v>0.42712181273602001</v>
+      </c>
+      <c r="D45">
+        <v>0.83100617484804096</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>75</v>
+      </c>
+      <c r="B46">
+        <v>0.33511760008532598</v>
+      </c>
+      <c r="C46">
+        <v>0.34295255355733001</v>
+      </c>
+      <c r="D46">
+        <v>0.61138563754668596</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>100</v>
+      </c>
+      <c r="B47">
+        <v>0.293647446400009</v>
+      </c>
+      <c r="C47">
+        <v>0.30112193312000801</v>
+      </c>
+      <c r="D47">
+        <v>0.50073379040002497</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>125</v>
+      </c>
+      <c r="B48">
+        <v>0.26942581447680702</v>
+      </c>
+      <c r="C48">
+        <v>0.276351956684803</v>
+      </c>
+      <c r="D48">
+        <v>0.43540864522237999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51">
+        <v>0.84415240404210501</v>
+      </c>
+      <c r="C51">
+        <v>0.86922567157892605</v>
+      </c>
+      <c r="D51">
+        <v>1.4410816506947</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>0.83039266569846104</v>
+      </c>
+      <c r="C52">
+        <v>0.82423927814735498</v>
+      </c>
+      <c r="D52">
+        <v>0.81864802279385096</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>0.81958879659789396</v>
+      </c>
+      <c r="C53">
+        <v>0.82641624535578395</v>
+      </c>
+      <c r="D53">
+        <v>0.82050771112420995</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54">
+        <v>75</v>
+      </c>
+      <c r="B54">
+        <v>0.82400235562666602</v>
+      </c>
+      <c r="C54">
+        <v>0.82478112954384797</v>
+      </c>
+      <c r="D54">
+        <v>0.81790866964210396</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55">
+        <v>100</v>
+      </c>
+      <c r="B55">
+        <v>0.82210387090526305</v>
+      </c>
+      <c r="C55">
+        <v>0.82702327194946701</v>
+      </c>
+      <c r="D55">
+        <v>0.81863543450947196</v>
+      </c>
+      <c r="G55" t="s">
+        <v>0</v>
+      </c>
+      <c r="H55" t="s">
+        <v>47</v>
+      </c>
+      <c r="I55" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56">
+        <v>125</v>
+      </c>
+      <c r="B56">
+        <v>0.82155425720589403</v>
+      </c>
+      <c r="C56">
+        <v>0.82419526552252398</v>
+      </c>
+      <c r="D56">
+        <v>0.82099782819031597</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56">
+        <v>1.52268029081602</v>
+      </c>
+      <c r="H56">
+        <v>1.43780074137608</v>
+      </c>
+      <c r="I56">
+        <f>C4*2</f>
+        <v>1.3660000000000001</v>
+      </c>
+      <c r="J56">
+        <f>D4*2</f>
+        <v>2.9820000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>1.6578541251368399</v>
+      </c>
+      <c r="H57">
+        <v>1.6296379385936799</v>
+      </c>
+      <c r="I57">
+        <f>C13*2</f>
+        <v>1.6479999999999999</v>
+      </c>
+      <c r="J57">
+        <f>D13*2</f>
+        <v>1.6379999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G58">
+        <v>1.16760149544421</v>
+      </c>
+      <c r="H58">
+        <v>0.93332297141894904</v>
+      </c>
+      <c r="I58">
+        <f>C22*2</f>
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="J58">
+        <f>D22*2</f>
+        <v>1.1279999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>0.66275949035789405</v>
+      </c>
+      <c r="C59">
+        <v>0.646769642778937</v>
+      </c>
+      <c r="D59">
+        <v>0.94681042576839702</v>
+      </c>
+      <c r="F59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59">
+        <v>1.13241640138105</v>
+      </c>
+      <c r="H59">
+        <v>0.97059486605473599</v>
+      </c>
+      <c r="I59">
+        <f>C31*2</f>
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="J59">
+        <f>D31*2</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>0.59821370318769196</v>
+      </c>
+      <c r="C60">
+        <v>0.55592109204209605</v>
+      </c>
+      <c r="D60">
+        <v>0.56395572194461696</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>0.57136774228210496</v>
+      </c>
+      <c r="C61">
+        <v>0.55974771792841505</v>
+      </c>
+      <c r="D61">
+        <v>0.55171826546526204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62">
+        <v>75</v>
+      </c>
+      <c r="B62">
+        <v>0.55748656215578896</v>
+      </c>
+      <c r="C62">
+        <v>0.55236330864279803</v>
+      </c>
+      <c r="D62">
+        <v>0.55422597434385901</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63">
+        <v>100</v>
+      </c>
+      <c r="B63">
+        <v>0.56159860690526298</v>
+      </c>
+      <c r="C63">
+        <v>0.55886010428630795</v>
+      </c>
+      <c r="D63">
+        <v>0.55105650762105196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64">
+        <v>125</v>
+      </c>
+      <c r="B64">
+        <v>0.55071846447157902</v>
+      </c>
+      <c r="C64">
+        <v>0.55782263785094499</v>
+      </c>
+      <c r="D64">
+        <v>0.55289256589473601</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67">
+        <v>0.59501313330526295</v>
+      </c>
+      <c r="C67">
+        <v>0.62319144353682998</v>
+      </c>
+      <c r="D67">
+        <v>0.56499037204210001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>25</v>
+      </c>
+      <c r="B68">
+        <v>0.569272978018461</v>
+      </c>
+      <c r="C68">
+        <v>0.56151460304841905</v>
+      </c>
+      <c r="D68">
+        <v>0.55231875150769105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>50</v>
+      </c>
+      <c r="B69">
+        <v>0.55530831087157795</v>
+      </c>
+      <c r="C69">
+        <v>0.55485058357893902</v>
+      </c>
+      <c r="D69">
+        <v>0.54882131907368303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>75</v>
+      </c>
+      <c r="B70">
+        <v>0.55049957566877195</v>
+      </c>
+      <c r="C70">
+        <v>0.55172049246315102</v>
+      </c>
+      <c r="D70">
+        <v>0.54218789692631497</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>100</v>
+      </c>
+      <c r="B71">
+        <v>0.55538468175157796</v>
+      </c>
+      <c r="C71">
+        <v>0.55496138543157303</v>
+      </c>
+      <c r="D71">
+        <v>0.54402908058947297</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>125</v>
+      </c>
+      <c r="B72">
+        <v>0.55466311382231503</v>
+      </c>
+      <c r="C72">
+        <v>0.555265802145679</v>
+      </c>
+      <c r="D72">
+        <v>0.54802852762947296</v>
       </c>
     </row>
   </sheetData>
@@ -38614,9 +39157,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -38624,7 +39167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -38638,7 +39181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -38655,7 +39198,7 @@
         <v>2.2741804224631399</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -38672,7 +39215,7 @@
         <v>1.4593802334631301</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -38689,7 +39232,7 @@
         <v>0.94015675940580301</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -38706,12 +39249,12 @@
         <v>0.77757128374857398</v>
       </c>
     </row>
-    <row r="43" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="13:15">
       <c r="M43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="13:15">
       <c r="N44" t="s">
         <v>19</v>
       </c>
@@ -38719,7 +39262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="13:15">
       <c r="M45">
         <v>32</v>
       </c>
@@ -38739,18 +39282,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F8BEC8-AEB5-3F4E-9605-35AFC868B601}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="49" workbookViewId="0">
+    <sheetView zoomScale="49" workbookViewId="0">
       <selection activeCell="E6" activeCellId="1" sqref="C6 E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -38764,7 +39307,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>4</v>
       </c>
@@ -38781,7 +39324,7 @@
         <v>1.4900916153600201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>8</v>
       </c>
@@ -38798,7 +39341,7 @@
         <v>2.15364379200004</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>16</v>
       </c>
@@ -38815,7 +39358,7 @@
         <v>2.8115508307199701</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>32</v>
       </c>
@@ -38832,12 +39375,12 @@
         <v>3.4696218393598999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -38851,7 +39394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>4</v>
       </c>
@@ -38868,7 +39411,7 @@
         <v>0.70050999142400605</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>8</v>
       </c>
@@ -38885,7 +39428,7 @@
         <v>0.96331392409602601</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>16</v>
       </c>
@@ -38902,7 +39445,7 @@
         <v>1.2274790507520399</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>32</v>
       </c>
@@ -38919,12 +39462,12 @@
         <v>1.4905966210560599</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -38938,7 +39481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>4</v>
       </c>
@@ -38955,7 +39498,7 @@
         <v>0.82387112586665501</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>8</v>
       </c>
@@ -38972,7 +39515,7 @@
         <v>1.0351484781714</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>16</v>
       </c>
@@ -38989,7 +39532,7 @@
         <v>1.2314947867428201</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>32</v>
       </c>
@@ -39006,12 +39549,12 @@
         <v>1.4251641732571101</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="C26" t="s">
         <v>21</v>
       </c>
@@ -39022,7 +39565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>4</v>
       </c>
@@ -39036,7 +39579,7 @@
         <v>0.81352163882666595</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>8</v>
       </c>
@@ -39050,7 +39593,7 @@
         <v>0.86948294783999902</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>16</v>
       </c>
@@ -39064,7 +39607,7 @@
         <v>0.81776230966857</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>32</v>
       </c>
@@ -39078,12 +39621,12 @@
         <v>0.81783354514286299</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>2</v>
       </c>
@@ -39097,7 +39640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>4</v>
       </c>
@@ -39114,7 +39657,7 @@
         <v>0.55197511771428498</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>8</v>
       </c>
@@ -39131,7 +39674,7 @@
         <v>0.66556407314284705</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>16</v>
       </c>
@@ -39148,7 +39691,7 @@
         <v>0.80861878994283998</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>32</v>
       </c>
@@ -39165,12 +39708,12 @@
         <v>0.96845884297140405</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="C42" t="s">
         <v>21</v>
       </c>
@@ -39181,7 +39724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4</v>
       </c>
@@ -39195,7 +39738,7 @@
         <v>0.55190261851428501</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>8</v>
       </c>
@@ -39209,7 +39752,7 @@
         <v>0.445015091382856</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>16</v>
       </c>
@@ -39223,7 +39766,7 @@
         <v>0.55276233307428402</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>32</v>
       </c>
@@ -39237,12 +39780,12 @@
         <v>0.55807887652571397</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="B50" t="s">
         <v>2</v>
       </c>
@@ -39256,7 +39799,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>4</v>
       </c>
@@ -39273,7 +39816,7 @@
         <v>0.49215105919999902</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>8</v>
       </c>
@@ -39290,7 +39833,7 @@
         <v>0.51584801737142805</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>16</v>
       </c>
@@ -39307,7 +39850,7 @@
         <v>0.55325926125714198</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>32</v>
       </c>
@@ -39324,12 +39867,12 @@
         <v>0.57934792822856496</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="C58" t="s">
         <v>21</v>
       </c>
@@ -39340,7 +39883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>4</v>
       </c>
@@ -39354,7 +39897,7 @@
         <v>0.49214442368</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>8</v>
       </c>
@@ -39368,7 +39911,7 @@
         <v>0.51583806409142796</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>16</v>
       </c>
@@ -39382,7 +39925,7 @@
         <v>0.53881741878857103</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>32</v>
       </c>
@@ -39406,13 +39949,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BF415F-BFDC-2641-9C46-18D0DFCE168E}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -39426,7 +39969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -39443,7 +39986,7 @@
         <v>2.0167691376641002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -39460,7 +40003,7 @@
         <v>0.95594155318864504</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -39477,7 +40020,7 @@
         <v>0.63770632137144401</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -39507,9 +40050,9 @@
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -39523,7 +40066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -39540,7 +40083,7 @@
         <v>1.7537265134080799</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -39557,7 +40100,7 @@
         <v>0.875961843565775</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -39574,7 +40117,7 @@
         <v>0.58144043958858005</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -39601,22 +40144,22 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>16</v>
       </c>
@@ -39624,7 +40167,7 @@
         <v>1.4529618815999901</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -39632,7 +40175,7 @@
         <v>1.4600360300799999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>64</v>
       </c>
@@ -39640,7 +40183,7 @@
         <v>1.4681880627200099</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>128</v>
       </c>
@@ -39648,7 +40191,7 @@
         <v>1.47102302208001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>256</v>
       </c>
@@ -39656,7 +40199,7 @@
         <v>1.91981266560005</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>512</v>
       </c>
@@ -39664,7 +40207,7 @@
         <v>3.4459279059199099</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>1024</v>
       </c>
@@ -39672,7 +40215,7 @@
         <v>6.6051643609595301</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>2048</v>
       </c>
@@ -39680,7 +40223,7 @@
         <v>12.951627436802401</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>4096</v>
       </c>
@@ -39688,7 +40231,7 @@
         <v>25.659261588490399</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>8192</v>
       </c>
@@ -39696,17 +40239,17 @@
         <v>33.954611500809897</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -39714,7 +40257,7 @@
         <v>0.62227649462855905</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -39722,7 +40265,7 @@
         <v>0.69468420022856103</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>64</v>
       </c>
@@ -39730,7 +40273,7 @@
         <v>0.70677023451427501</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>128</v>
       </c>
@@ -39738,7 +40281,7 @@
         <v>0.72407198628570402</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>256</v>
       </c>
@@ -39746,7 +40289,7 @@
         <v>0.71945108571427596</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>512</v>
       </c>
@@ -39754,7 +40297,7 @@
         <v>0.71579552457141804</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>1024</v>
       </c>
@@ -39762,7 +40305,7 @@
         <v>0.71196466194284702</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>2048</v>
       </c>
@@ -39770,7 +40313,7 @@
         <v>0.69591278719998895</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>4096</v>
       </c>
@@ -39778,7 +40321,7 @@
         <v>0.71578731885713198</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>8192</v>
       </c>
@@ -39800,14 +40343,14 @@
       <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -39818,7 +40361,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>100</v>
       </c>
@@ -39832,7 +40375,7 @@
         <v>0.56583017343999498</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>200</v>
       </c>
@@ -39846,7 +40389,7 @@
         <v>0.68198290559999297</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>400</v>
       </c>
@@ -39860,7 +40403,7 @@
         <v>0.88295811071998898</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>800</v>
       </c>
@@ -39874,7 +40417,7 @@
         <v>1.15122825343999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1600</v>
       </c>
@@ -39888,7 +40431,7 @@
         <v>1.54958330752002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>3200</v>
       </c>
@@ -39902,7 +40445,7 @@
         <v>2.3523447827200199</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>6400</v>
       </c>
@@ -39916,12 +40459,12 @@
         <v>3.4689794035199002</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -39932,7 +40475,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>100</v>
       </c>
@@ -39946,7 +40489,7 @@
         <v>0.32949495654399702</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>200</v>
       </c>
@@ -39960,7 +40503,7 @@
         <v>0.37655983948799598</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>400</v>
       </c>
@@ -39974,7 +40517,7 @@
         <v>0.45622986265599202</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>800</v>
       </c>
@@ -39988,7 +40531,7 @@
         <v>0.56335831091199595</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>1600</v>
       </c>
@@ -40002,7 +40545,7 @@
         <v>0.72320312166400802</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>3200</v>
       </c>
@@ -40016,7 +40559,7 @@
         <v>1.0434028654080301</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>6400</v>
       </c>
@@ -40030,12 +40573,12 @@
         <v>1.4905693281280601</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -40046,7 +40589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>100</v>
       </c>
@@ -40060,7 +40603,7 @@
         <v>0.25080902796799598</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>200</v>
       </c>
@@ -40074,7 +40617,7 @@
         <v>0.27402011993599801</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>400</v>
       </c>
@@ -40088,7 +40631,7 @@
         <v>0.31364528857600199</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>800</v>
       </c>
@@ -40102,7 +40645,7 @@
         <v>0.36703585036800601</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>1600</v>
       </c>
@@ -40116,7 +40659,7 @@
         <v>0.44695445926401201</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>3200</v>
       </c>
@@ -40130,7 +40673,7 @@
         <v>0.60745929190402403</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>6400</v>
       </c>
@@ -40144,12 +40687,12 @@
         <v>0.83018577292803997</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -40160,7 +40703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>100</v>
       </c>
@@ -40174,7 +40717,7 @@
         <v>0.224133521919997</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>200</v>
       </c>
@@ -40188,7 +40731,7 @@
         <v>0.239455191722663</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>400</v>
       </c>
@@ -40202,7 +40745,7 @@
         <v>0.26624995097599502</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>800</v>
       </c>
@@ -40216,7 +40759,7 @@
         <v>0.30195340927999398</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>1600</v>
       </c>
@@ -40230,7 +40773,7 @@
         <v>0.35511338606932502</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>3200</v>
       </c>
@@ -40244,7 +40787,7 @@
         <v>0.46193100603732101</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>6400</v>
       </c>
@@ -40258,12 +40801,12 @@
         <v>0.61128305928535198</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -40274,7 +40817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>100</v>
       </c>
@@ -40288,7 +40831,7 @@
         <v>0.21139137612800299</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>200</v>
       </c>
@@ -40302,7 +40845,7 @@
         <v>0.223161735680004</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>400</v>
       </c>
@@ -40316,7 +40859,7 @@
         <v>0.24290003929600601</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>800</v>
       </c>
@@ -40330,7 +40873,7 @@
         <v>0.26937500736000702</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>1600</v>
       </c>
@@ -40344,7 +40887,7 @@
         <v>0.30939158668800998</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>3200</v>
       </c>
@@ -40358,7 +40901,7 @@
         <v>0.38961193132801603</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>6400</v>
       </c>
@@ -40372,12 +40915,12 @@
         <v>0.501487123776025</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -40388,7 +40931,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>100</v>
       </c>
@@ -40402,7 +40945,7 @@
         <v>0.20750442367999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>200</v>
       </c>
@@ -40416,7 +40959,7 @@
         <v>0.21273843932160499</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>400</v>
       </c>
@@ -40430,7 +40973,7 @@
         <v>0.22841034695680701</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>800</v>
       </c>
@@ -40444,7 +40987,7 @@
         <v>0.24972326727680999</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>1600</v>
       </c>
@@ -40458,7 +41001,7 @@
         <v>0.28192298086400502</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>3200</v>
       </c>
@@ -40472,7 +41015,7 @@
         <v>0.34577728358399501</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>6400</v>
       </c>
@@ -40497,20 +41040,20 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -40518,7 +41061,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -40529,7 +41072,7 @@
         <v>78.412617753446298</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -40540,7 +41083,7 @@
         <v>42.640659457852998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -40551,7 +41094,7 @@
         <v>42.115842916466697</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -40562,7 +41105,7 @@
         <v>3.6601920153598102</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -40571,7 +41114,7 @@
         <v>67.908423001619795</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -40580,12 +41123,12 @@
         <v>6.9392436787197997</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>26</v>
       </c>
@@ -40593,7 +41136,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -40604,7 +41147,7 @@
         <v>17.382887367320802</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -40615,7 +41158,7 @@
         <v>14.675562218525</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -40626,7 +41169,7 @@
         <v>13.230031857829699</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -40637,7 +41180,7 @@
         <v>1.6224625421714201</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -40646,7 +41189,7 @@
         <v>2.0758292571428201</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -40655,12 +41198,12 @@
         <v>2.8503283465142202</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -40668,7 +41211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -40679,7 +41222,7 @@
         <v>12.1320219355473</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -40690,7 +41233,7 @@
         <v>9.2510466153192201</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -40701,7 +41244,7 @@
         <v>9.1911636123425904</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -40712,7 +41255,7 @@
         <v>0.96216006765714301</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -40721,7 +41264,7 @@
         <v>1.6534550326856861</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -40730,12 +41273,12 @@
         <v>1.9369176859428081</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -40743,7 +41286,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -40754,7 +41297,7 @@
         <v>8.2827718244604895</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -40765,7 +41308,7 @@
         <v>5.2856826016025202</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -40776,7 +41319,7 @@
         <v>4.6834424813715598</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -40787,7 +41330,7 @@
         <v>1.0365232265142801</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -40796,7 +41339,7 @@
         <v>1.3903103506285539</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -40805,7 +41348,7 @@
         <v>1.1586958564571299</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="21" customHeight="1">
       <c r="B39" t="s">
         <v>28</v>
       </c>

</xml_diff>